<commit_message>
updated readme with small description
</commit_message>
<xml_diff>
--- a/task_list/BigData_Fall2017_TaskList.xlsx
+++ b/task_list/BigData_Fall2017_TaskList.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
   <si>
     <t>Big Data Analytics Project Task List</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Team Members:</t>
   </si>
   <si>
-    <t xml:space="preserve">4) </t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
   </si>
   <si>
     <t>Plan where data will reside</t>
-  </si>
-  <si>
-    <t>Data Source 1 Processing</t>
   </si>
   <si>
     <t>Write code to ingest data source 1</t>
@@ -146,9 +140,6 @@
     <t>Write code to clean/format (ETL) data source 1</t>
   </si>
   <si>
-    <t>Data Source 2 Processing</t>
-  </si>
-  <si>
     <t>Write code to ingest data source 2</t>
   </si>
   <si>
@@ -156,9 +147,6 @@
   </si>
   <si>
     <t>Write code to clean/format (ETL) data source 2</t>
-  </si>
-  <si>
-    <t>Data Source 3 Processing</t>
   </si>
   <si>
     <t>Write code to ingest data source 3</t>
@@ -245,9 +233,6 @@
     <t>oct/27</t>
   </si>
   <si>
-    <t>• We will initialy save about 250GB of data</t>
-  </si>
-  <si>
     <t>• We will save it on Dumbo</t>
   </si>
   <si>
@@ -258,13 +243,28 @@
   </si>
   <si>
     <t>oct/31</t>
+  </si>
+  <si>
+    <t>• We will initialy have about 250GB of data</t>
+  </si>
+  <si>
+    <t>•In this step, you'll read the data from the source and write it or copy it into HDFS</t>
+  </si>
+  <si>
+    <t>Taxi Rides Processing</t>
+  </si>
+  <si>
+    <t>NYPD Crimes Processing</t>
+  </si>
+  <si>
+    <t>Weather data Processing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -317,6 +317,18 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -350,7 +362,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -597,51 +609,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="10"/>
       </left>
       <right style="thin">
@@ -695,10 +662,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -710,13 +681,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -749,6 +720,45 @@
     <xf numFmtId="15" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -758,6 +768,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -776,15 +792,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -794,12 +801,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -810,52 +811,17 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2041,10 +2007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2060,634 +2026,623 @@
   <sheetData>
     <row r="1" spans="1:6" ht="81" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="43"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37"/>
+      <c r="C3" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="49"/>
+      <c r="C5" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="41"/>
+    </row>
+    <row r="6" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38"/>
+    </row>
+    <row r="7" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="38"/>
+    </row>
+    <row r="9" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
+    </row>
+    <row r="10" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="52"/>
-    </row>
-    <row r="7" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
-    </row>
-    <row r="8" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23"/>
-    </row>
-    <row r="10" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
-    </row>
-    <row r="11" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
+    </row>
+    <row r="14" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33"/>
+    </row>
+    <row r="15" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="44" t="s">
+      <c r="D15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="13" t="s">
+      <c r="F15" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
-    </row>
-    <row r="15" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="18" t="s">
+    <row r="16" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
+    </row>
+    <row r="22" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
+    </row>
+    <row r="23" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20"/>
-    </row>
-    <row r="16" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="10" t="s">
+    </row>
+    <row r="24" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="38"/>
+    </row>
+    <row r="30" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="7"/>
+      <c r="B30" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="33"/>
+    </row>
+    <row r="31" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="14" t="s">
+      <c r="F31" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="33" t="s">
+    <row r="33" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="12" t="s">
+    </row>
+    <row r="34" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="15" t="s">
+    <row r="35" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="23"/>
-    </row>
-    <row r="23" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
-    </row>
-    <row r="24" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="8" t="s">
+    <row r="36" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="23"/>
-    </row>
-    <row r="31" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="20"/>
-    </row>
-    <row r="32" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="11"/>
+      <c r="C36" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="38"/>
     </row>
     <row r="38" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="23"/>
-    </row>
-    <row r="39" spans="1:6" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="23"/>
-    </row>
-    <row r="40" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
-      <c r="B40" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="20"/>
-    </row>
-    <row r="41" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="36"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="38"/>
+    </row>
+    <row r="39" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="7"/>
+      <c r="B39" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
+    </row>
+    <row r="40" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="11"/>
+    </row>
+    <row r="41" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="11"/>
+    </row>
+    <row r="43" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" s="11"/>
-    </row>
-    <row r="43" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="8" t="s">
+    </row>
+    <row r="45" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="11"/>
-    </row>
-    <row r="44" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="33" t="s">
+      <c r="C45" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E47" s="17"/>
-      <c r="F47" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="17"/>
+      <c r="F46" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="35">
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="C3:F3"/>
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="E25:E28"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="D25:D28"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="D32:D35"/>
     <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B6:F6"/>
     <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B29:F29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>